<commit_message>
typology of 7 factor - 3 clusters
</commit_message>
<xml_diff>
--- a/results/df-fa-five-cluster-rank.xlsx
+++ b/results/df-fa-five-cluster-rank.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,40 +365,50 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>dugwell</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>spring</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>well</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>piped_to_yard_tap</t>
+          <t>piped_home</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>piped_to_dwelling</t>
+          <t>piped_yard_tap</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>natural_commodity</t>
+          <t>cheap_commercial</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>surface_water</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>thirthy_min_less_travel</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>norm</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>distToCentroid</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>clusters</t>
         </is>
@@ -411,28 +421,36 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.37860810547924</v>
+        <v>0.5724182174237744</v>
       </c>
       <c r="C2">
-        <v>0.6054630982421287</v>
+        <v>0.2794850470029633</v>
       </c>
       <c r="D2">
-        <v>0.4398335349144496</v>
+        <v>0.4740641704232623</v>
       </c>
       <c r="E2">
-        <v>0.5169148237810761</v>
+        <v>0.489052694026701</v>
       </c>
       <c r="F2">
-        <v>0.3941816894808592</v>
+        <v>0.3327189831430472</v>
       </c>
       <c r="G2">
-        <v>1.06111419680894</v>
+        <v>0.6406390153077257</v>
       </c>
       <c r="H2">
-        <v>0.3643947795683522</v>
+        <v>0.5244550455963321</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>1.290680923729942</v>
+      </c>
+      <c r="J2">
+        <v>0.2463713788039732</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -442,28 +460,36 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.1374996930512995</v>
+        <v>0.1733472865487872</v>
       </c>
       <c r="C3">
-        <v>0.167962452359574</v>
+        <v>0.1663123431465754</v>
       </c>
       <c r="D3">
-        <v>0.1735878432854467</v>
+        <v>0.7812554899521552</v>
       </c>
       <c r="E3">
-        <v>0.8503784878760169</v>
+        <v>0.2160445733788369</v>
       </c>
       <c r="F3">
-        <v>0.3456189962439017</v>
+        <v>0.3179486671870097</v>
       </c>
       <c r="G3">
-        <v>0.9590862075618019</v>
+        <v>0.266875599494618</v>
       </c>
       <c r="H3">
-        <v>1.246491237716195</v>
+        <v>0.5813036444273134</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1.10678468687439</v>
+      </c>
+      <c r="J3">
+        <v>1.052121795405808</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -473,28 +499,36 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.4238036002360227</v>
+        <v>0.5554028955061096</v>
       </c>
       <c r="C4">
-        <v>0.6233491942818576</v>
+        <v>0.2656793476606521</v>
       </c>
       <c r="D4">
-        <v>0.513843161594323</v>
+        <v>0.6221088232475103</v>
       </c>
       <c r="E4">
-        <v>0.6639955978161501</v>
+        <v>0.5179950423562272</v>
       </c>
       <c r="F4">
-        <v>0.4389020612811098</v>
+        <v>0.4010243884503956</v>
       </c>
       <c r="G4">
-        <v>1.210674885185176</v>
+        <v>0.8739405228768782</v>
       </c>
       <c r="H4">
-        <v>0.2148340911921167</v>
+        <v>0.4280040402932476</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>1.463617504727127</v>
+      </c>
+      <c r="J4">
+        <v>0.07343479780678885</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -504,28 +538,36 @@
         </is>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.006249718744720773</v>
       </c>
       <c r="C5">
-        <v>0.002252355435700771</v>
+        <v>0.01802207152283934</v>
       </c>
       <c r="D5">
-        <v>0.1151603776093063</v>
+        <v>0.9992766213025949</v>
       </c>
       <c r="E5">
-        <v>0.9899717593177034</v>
+        <v>0.05567089370361541</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.9966499234549289</v>
+        <v>0.197841302168221</v>
       </c>
       <c r="H5">
-        <v>1.208927521823068</v>
+        <v>0.5088644593045378</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>1.140219753872458</v>
+      </c>
+      <c r="J5">
+        <v>2.017680672556671</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -535,28 +577,36 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.215702034261702</v>
+        <v>0.1723055432036395</v>
       </c>
       <c r="C6">
-        <v>0.204107962069363</v>
+        <v>0.1720940566035091</v>
       </c>
       <c r="D6">
-        <v>0.4847073028764705</v>
+        <v>0.694623742899713</v>
       </c>
       <c r="E6">
-        <v>0.7011007892548125</v>
+        <v>0.4169395223522535</v>
       </c>
       <c r="F6">
-        <v>0.2276693341145948</v>
+        <v>0.2060015659171007</v>
       </c>
       <c r="G6">
-        <v>0.9308620948435012</v>
+        <v>0.4634648493769318</v>
       </c>
       <c r="H6">
-        <v>2.239946144093491</v>
+        <v>0.4247651654227611</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>1.07392179955581</v>
+      </c>
+      <c r="J6">
+        <v>2.083978626873319</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -566,28 +616,36 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.08900232835183163</v>
+        <v>0.1165068306841544</v>
       </c>
       <c r="C7">
-        <v>0.1645338754891485</v>
+        <v>0.08746231304577737</v>
       </c>
       <c r="D7">
-        <v>0.2832823480296564</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.2916840047778304</v>
       </c>
       <c r="F7">
-        <v>0.1961306655599404</v>
+        <v>0.1829046315901536</v>
       </c>
       <c r="G7">
-        <v>0.3920573138122874</v>
+        <v>0.1907371042350997</v>
       </c>
       <c r="H7">
-        <v>1.033451662565005</v>
+        <v>0.5876123519242676</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0.722098386486016</v>
+      </c>
+      <c r="J7">
+        <v>1.436808095794182</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -597,28 +655,36 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.3093180729486195</v>
+        <v>0.6379424323621061</v>
       </c>
       <c r="C8">
-        <v>0.6844461019025947</v>
+        <v>0.2113416584498435</v>
       </c>
       <c r="D8">
-        <v>0.4443813812544071</v>
+        <v>0.4559905229898179</v>
       </c>
       <c r="E8">
-        <v>0.472057968262336</v>
+        <v>0.4926719990226089</v>
       </c>
       <c r="F8">
-        <v>0.3025271873449032</v>
+        <v>0.2827229550925449</v>
       </c>
       <c r="G8">
-        <v>1.037294737840052</v>
+        <v>0.4847494615158167</v>
       </c>
       <c r="H8">
-        <v>0.3882142385372407</v>
+        <v>0.6788341526241041</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>1.295383733040867</v>
+      </c>
+      <c r="J8">
+        <v>0.2416685694930483</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -628,28 +694,36 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.08511927867502257</v>
+        <v>0.07837501558407362</v>
       </c>
       <c r="C9">
-        <v>0.1758744175001936</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0.8103062340605804</v>
       </c>
       <c r="E9">
-        <v>0.7536284139039488</v>
+        <v>0.7530348752463829</v>
       </c>
       <c r="F9">
-        <v>0.1800460246538417</v>
+        <v>0.2450488351586027</v>
       </c>
       <c r="G9">
-        <v>1.280058381313221</v>
+        <v>0.4310157306709256</v>
       </c>
       <c r="H9">
-        <v>1.890749857623772</v>
+        <v>0.3901205326871015</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>1.275859663554353</v>
+      </c>
+      <c r="J9">
+        <v>1.882040762874776</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -659,28 +733,36 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.332389631708566</v>
+        <v>0.6692561320068629</v>
       </c>
       <c r="C10">
-        <v>0.6862942233977999</v>
+        <v>0.2893428261258724</v>
       </c>
       <c r="D10">
-        <v>0.5700352398587129</v>
+        <v>0.3422915527134101</v>
       </c>
       <c r="E10">
-        <v>0.348112878379525</v>
+        <v>0.512445193102183</v>
       </c>
       <c r="F10">
-        <v>0.1540055389176266</v>
+        <v>0.217836510973845</v>
       </c>
       <c r="G10">
-        <v>1.025340472783705</v>
+        <v>0.214987050208431</v>
       </c>
       <c r="H10">
-        <v>0.4001685035935874</v>
+        <v>0.786722774548546</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>1.274359260772145</v>
+      </c>
+      <c r="J10">
+        <v>0.2626930417617703</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -690,28 +772,36 @@
         </is>
       </c>
       <c r="B11">
+        <v>0.51321879163111</v>
+      </c>
+      <c r="C11">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>0.4081622990211214</v>
-      </c>
       <c r="D11">
-        <v>0.6014436151565805</v>
+        <v>0.4670299707543935</v>
       </c>
       <c r="E11">
-        <v>0.4777808154990012</v>
+        <v>0.6389302771744395</v>
       </c>
       <c r="F11">
-        <v>0.1743640335817195</v>
+        <v>0.1850743412739337</v>
       </c>
       <c r="G11">
-        <v>1.336790263437239</v>
+        <v>0.3059030329285412</v>
       </c>
       <c r="H11">
-        <v>0.08871871294005396</v>
+        <v>0.8152177753017932</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>1.637727577858179</v>
+      </c>
+      <c r="J11">
+        <v>0.1006752753242637</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -721,28 +811,36 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.1477545930019207</v>
+        <v>0.4295485388568042</v>
       </c>
       <c r="C12">
-        <v>0.3914328662551107</v>
+        <v>0.197443628292338</v>
       </c>
       <c r="D12">
-        <v>0.2275245166450688</v>
+        <v>0.3810489406372295</v>
       </c>
       <c r="E12">
-        <v>0.5740804420259595</v>
+        <v>0.2736086784754569</v>
       </c>
       <c r="F12">
-        <v>0.5879489798367857</v>
+        <v>0.3969322318777774</v>
       </c>
       <c r="G12">
-        <v>0.9497741157876777</v>
+        <v>0.3684485149057752</v>
       </c>
       <c r="H12">
-        <v>3.122380179210631</v>
+        <v>0.08083012878688521</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>0.8622058641905357</v>
+      </c>
+      <c r="J12">
+        <v>2.295694562238594</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -752,28 +850,36 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.3999182024227658</v>
+        <v>0.4660733409872863</v>
       </c>
       <c r="C13">
-        <v>0.4990248681285047</v>
+        <v>0.3182658361163819</v>
       </c>
       <c r="D13">
-        <v>0.4715324493235238</v>
+        <v>0.4371264428772796</v>
       </c>
       <c r="E13">
-        <v>0.4278911701172217</v>
+        <v>0.4578648761742926</v>
       </c>
       <c r="F13">
-        <v>0.2327401648041904</v>
+        <v>0.2785909264162509</v>
       </c>
       <c r="G13">
-        <v>0.9319667784755722</v>
+        <v>0.5085118771559029</v>
       </c>
       <c r="H13">
-        <v>0.4935421979017204</v>
+        <v>0.7522440912674003</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>1.273305022314511</v>
+      </c>
+      <c r="J13">
+        <v>0.2637472802194045</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -783,28 +889,36 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.3240012589151352</v>
+        <v>0.8541269165162611</v>
       </c>
       <c r="C14">
-        <v>0.9013835985839157</v>
+        <v>0.2146152743279821</v>
       </c>
       <c r="D14">
-        <v>0.501580903318618</v>
+        <v>0.4194341369462211</v>
       </c>
       <c r="E14">
-        <v>0.4537853914681756</v>
+        <v>0.4127746554413343</v>
       </c>
       <c r="F14">
-        <v>0.2244257712409631</v>
+        <v>0.3059885881945644</v>
       </c>
       <c r="G14">
-        <v>1.19387634135853</v>
+        <v>0.5179273079629756</v>
       </c>
       <c r="H14">
-        <v>0.2316326350187625</v>
+        <v>0.7088980184348626</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>1.409366712350954</v>
+      </c>
+      <c r="J14">
+        <v>0.1276855901829612</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -814,28 +928,36 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.02214741325687635</v>
+        <v>0.0443809265296003</v>
       </c>
       <c r="C15">
-        <v>0.06070090218618214</v>
+        <v>0.01828674723077807</v>
       </c>
       <c r="D15">
-        <v>0.005798361109362105</v>
+        <v>0.9356765848623616</v>
       </c>
       <c r="E15">
-        <v>0.9661084885977459</v>
+        <v>0.001934996035546409</v>
       </c>
       <c r="F15">
-        <v>0.1256519970519421</v>
+        <v>0.1125957195317144</v>
       </c>
       <c r="G15">
-        <v>0.9764029724122638</v>
+        <v>0.271437014775242</v>
       </c>
       <c r="H15">
-        <v>1.229174472865733</v>
+        <v>0.4699816160132052</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>1.088594073045872</v>
+      </c>
+      <c r="J15">
+        <v>2.069306353383257</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -845,28 +967,36 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.2929136248849009</v>
+        <v>0.3351042098192096</v>
       </c>
       <c r="C16">
-        <v>0.3558187756388855</v>
+        <v>0.2594990989664349</v>
       </c>
       <c r="D16">
-        <v>0.6239621852513133</v>
+        <v>0.685069466047686</v>
       </c>
       <c r="E16">
-        <v>0.708191628235378</v>
+        <v>0.7267405520646687</v>
       </c>
       <c r="F16">
-        <v>0.3918664099074576</v>
+        <v>0.2443217375584422</v>
       </c>
       <c r="G16">
-        <v>1.121083791195108</v>
+        <v>0.2973789334200525</v>
       </c>
       <c r="H16">
-        <v>2.049724447741884</v>
+        <v>0.4457287043673597</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>1.234466701256741</v>
+      </c>
+      <c r="J16">
+        <v>1.923433725172388</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -876,28 +1006,36 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.4766704329092389</v>
+        <v>0.4432752500520991</v>
       </c>
       <c r="C17">
-        <v>0.5061929402201787</v>
+        <v>0.3781890881573893</v>
       </c>
       <c r="D17">
-        <v>0.727603233245901</v>
+        <v>0.5558611044646034</v>
       </c>
       <c r="E17">
-        <v>0.5509206960866621</v>
+        <v>0.7025442682839119</v>
       </c>
       <c r="F17">
-        <v>0.2510256000460155</v>
+        <v>0.2779946853302961</v>
       </c>
       <c r="G17">
-        <v>1.174470061186574</v>
+        <v>0.3513378091470828</v>
       </c>
       <c r="H17">
-        <v>0.2510389151907189</v>
+        <v>0.6050517848829414</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>1.307240189736932</v>
+      </c>
+      <c r="J17">
+        <v>0.2298121127969834</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -907,28 +1045,36 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.8870157516400352</v>
+        <v>0.5383770533433352</v>
       </c>
       <c r="C18">
-        <v>0.5310671660662611</v>
+        <v>0.7846187970680508</v>
       </c>
       <c r="D18">
-        <v>0.605318646122783</v>
+        <v>0.4644728464434113</v>
       </c>
       <c r="E18">
-        <v>0.5049481696481608</v>
+        <v>0.4415804765641568</v>
       </c>
       <c r="F18">
-        <v>0.1951674922477848</v>
+        <v>0.3155324632506825</v>
       </c>
       <c r="G18">
-        <v>1.314649362353484</v>
+        <v>0.74425542003652</v>
       </c>
       <c r="H18">
-        <v>0.1108596140238085</v>
+        <v>0.5511106196493014</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>1.507781360593789</v>
+      </c>
+      <c r="J18">
+        <v>0.02927094194012647</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -938,28 +1084,36 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.3016676406506052</v>
+        <v>0.5441322407346009</v>
       </c>
       <c r="C19">
-        <v>0.5951416512261936</v>
+        <v>0.2071726258044386</v>
       </c>
       <c r="D19">
-        <v>0.6595111317983502</v>
+        <v>0.6270585487207295</v>
       </c>
       <c r="E19">
-        <v>0.6136773804535081</v>
+        <v>0.6137474030508897</v>
       </c>
       <c r="F19">
-        <v>0.2515738801294872</v>
+        <v>0.2735714339530418</v>
       </c>
       <c r="G19">
-        <v>1.148930471286043</v>
+        <v>0.4844009312793265</v>
       </c>
       <c r="H19">
-        <v>0.2765785050912495</v>
+        <v>0.6695057342429037</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>1.366240173047387</v>
+      </c>
+      <c r="J19">
+        <v>0.1708121294865281</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -969,28 +1123,36 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.08929942417124334</v>
+        <v>0.04054530053760146</v>
       </c>
       <c r="C20">
-        <v>0.06099100307554368</v>
+        <v>0.1797787517104879</v>
       </c>
       <c r="D20">
-        <v>0.1345893110940799</v>
+        <v>0.4866491836088315</v>
       </c>
       <c r="E20">
-        <v>0.7489241815835165</v>
+        <v>0.2755531883903987</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>1.261227973855161</v>
+        <v>0.02793189015429641</v>
       </c>
       <c r="H20">
-        <v>2.810926321143147</v>
+        <v>0.520796934334671</v>
       </c>
       <c r="I20">
-        <v>4</v>
+        <v>1.272293576892341</v>
+      </c>
+      <c r="J20">
+        <v>0.8866129053878575</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1000,28 +1162,36 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.01704204529686534</v>
+        <v>0.04700321659942933</v>
       </c>
       <c r="C21">
-        <v>0.04020883123023998</v>
+        <v>0.03542452273518945</v>
       </c>
       <c r="D21">
-        <v>0.00334844095506473</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0.01943771407366398</v>
+        <v>0.01232009601457685</v>
       </c>
       <c r="G21">
-        <v>1.001147450779375</v>
+        <v>0.1791549781404083</v>
       </c>
       <c r="H21">
-        <v>1.204429994498621</v>
+        <v>0.5729327576553055</v>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>1.167888879532004</v>
+      </c>
+      <c r="J21">
+        <v>1.990011546897125</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1031,28 +1201,36 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.3694121470196452</v>
+        <v>0.8483580494627152</v>
       </c>
       <c r="C22">
-        <v>0.8157388778551036</v>
+        <v>0.356067984877925</v>
       </c>
       <c r="D22">
-        <v>0.3815373101559206</v>
+        <v>0.6194420629368137</v>
       </c>
       <c r="E22">
-        <v>0.7534731314217225</v>
+        <v>0.4495238077636043</v>
       </c>
       <c r="F22">
-        <v>0.365444888750621</v>
+        <v>0.2435485894751917</v>
       </c>
       <c r="G22">
-        <v>1.284031812977931</v>
+        <v>0.2015001882559833</v>
       </c>
       <c r="H22">
-        <v>0.1414771633993615</v>
+        <v>0.3856327935180525</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>1.296497900408637</v>
+      </c>
+      <c r="J22">
+        <v>0.2405544021252786</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1062,28 +1240,36 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.3663075935433198</v>
+        <v>0.417728103008857</v>
       </c>
       <c r="C23">
-        <v>0.5092059063090556</v>
+        <v>0.2219139212636367</v>
       </c>
       <c r="D23">
-        <v>0.6672520940790505</v>
+        <v>0.6785416612327249</v>
       </c>
       <c r="E23">
-        <v>0.6477240416632806</v>
+        <v>0.5705459126579124</v>
       </c>
       <c r="F23">
-        <v>0.1943262334115918</v>
+        <v>0.2714444594435935</v>
       </c>
       <c r="G23">
-        <v>1.138422761675536</v>
+        <v>0.5840193117140726</v>
       </c>
       <c r="H23">
-        <v>0.2870862147017566</v>
+        <v>0.6040330919216308</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>1.33764741547506</v>
+      </c>
+      <c r="J23">
+        <v>0.1994048870588556</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1093,28 +1279,36 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.6788833240144442</v>
+        <v>0.488967515827357</v>
       </c>
       <c r="C24">
-        <v>0.5133104331897724</v>
+        <v>0.5777114138662979</v>
       </c>
       <c r="D24">
-        <v>0.6670191170111786</v>
+        <v>0.4704111116038663</v>
       </c>
       <c r="E24">
-        <v>0.4810217401803793</v>
+        <v>0.5570058911626871</v>
       </c>
       <c r="F24">
-        <v>0.2028855381819477</v>
+        <v>0.2871425252800607</v>
       </c>
       <c r="G24">
-        <v>1.200761894396339</v>
+        <v>0.5684910567859367</v>
       </c>
       <c r="H24">
-        <v>0.2247470819809541</v>
+        <v>0.5936216115031062</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>1.364698287193709</v>
+      </c>
+      <c r="J24">
+        <v>0.1723540153402059</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1124,28 +1318,36 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.2570996449400474</v>
+        <v>0.2043240669166619</v>
       </c>
       <c r="C25">
-        <v>0.2606618198320522</v>
+        <v>0.193265168964434</v>
       </c>
       <c r="D25">
-        <v>0.8271645984304589</v>
+        <v>0.774366220640183</v>
       </c>
       <c r="E25">
-        <v>0.7266637131122983</v>
+        <v>0.7212242535678695</v>
       </c>
       <c r="F25">
-        <v>0.1642703575284754</v>
+        <v>0.1976586589293624</v>
       </c>
       <c r="G25">
-        <v>1.171866454405008</v>
+        <v>0.2727598583257055</v>
       </c>
       <c r="H25">
-        <v>1.998941784531985</v>
+        <v>0.5672443421207263</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>1.278334950977597</v>
+      </c>
+      <c r="J25">
+        <v>1.879565475451532</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1155,28 +1357,36 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.3225016071042833</v>
+        <v>0.4274660574404323</v>
       </c>
       <c r="C26">
-        <v>0.4987421398758482</v>
+        <v>0.2267548409431511</v>
       </c>
       <c r="D26">
-        <v>0.9431844467959191</v>
+        <v>0.6696732907740834</v>
       </c>
       <c r="E26">
-        <v>0.5860268121421215</v>
+        <v>0.9295148793548888</v>
       </c>
       <c r="F26">
-        <v>0.2116469931199755</v>
+        <v>0.2373012252752822</v>
       </c>
       <c r="G26">
-        <v>1.276937658461326</v>
+        <v>0.2826542023960937</v>
       </c>
       <c r="H26">
-        <v>0.1485713179159667</v>
+        <v>0.8222131910896445</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>1.535853188532121</v>
+      </c>
+      <c r="J26">
+        <v>0.001199114001794399</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1186,28 +1396,36 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.3909169092278594</v>
+        <v>0.4597191743275593</v>
       </c>
       <c r="C27">
-        <v>0.4826834361319597</v>
+        <v>0.3072953766897908</v>
       </c>
       <c r="D27">
-        <v>0.4178154235845504</v>
+        <v>0.4971563506898161</v>
       </c>
       <c r="E27">
-        <v>0.510216187373979</v>
+        <v>0.6019185337715229</v>
       </c>
       <c r="F27">
-        <v>0.4239481658454889</v>
+        <v>0.2959176632989249</v>
       </c>
       <c r="G27">
-        <v>1.000210809181619</v>
+        <v>0.5079102611581778</v>
       </c>
       <c r="H27">
-        <v>0.4252981671956737</v>
+        <v>0.6296609084345071</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>1.287344352751369</v>
+      </c>
+      <c r="J27">
+        <v>0.2497079497825461</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1217,28 +1435,36 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.1395316285303666</v>
+        <v>0.03322447050908708</v>
       </c>
       <c r="C28">
-        <v>0.07945423171343025</v>
+        <v>0.1427549330337106</v>
       </c>
       <c r="D28">
-        <v>0.5907108668870076</v>
+        <v>0.6771961774472386</v>
       </c>
       <c r="E28">
-        <v>0.7495124813045958</v>
+        <v>0.5396847772241048</v>
       </c>
       <c r="F28">
-        <v>0.4848277265769483</v>
+        <v>0.491587579065452</v>
       </c>
       <c r="G28">
-        <v>1.082380830689943</v>
+        <v>0.2200520633411587</v>
       </c>
       <c r="H28">
-        <v>2.989773464308366</v>
+        <v>0.4327300661209997</v>
       </c>
       <c r="I28">
-        <v>4</v>
+        <v>1.117440703777999</v>
+      </c>
+      <c r="J28">
+        <v>1.041465778502199</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1248,28 +1474,36 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.3749329728563592</v>
+        <v>0.4470807868297426</v>
       </c>
       <c r="C29">
-        <v>0.4639869387716651</v>
+        <v>0.3260933623543778</v>
       </c>
       <c r="D29">
-        <v>0.4348450216997136</v>
+        <v>0.3030951792755465</v>
       </c>
       <c r="E29">
-        <v>0.3322132272591632</v>
+        <v>0.3357363163565129</v>
       </c>
       <c r="F29">
-        <v>0.1961717315185454</v>
+        <v>0.2577098804870205</v>
       </c>
       <c r="G29">
-        <v>0.8329452460969841</v>
+        <v>0.4548376351702116</v>
       </c>
       <c r="H29">
-        <v>0.5925637302803085</v>
+        <v>0.5948362428152971</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>1.066735902357789</v>
+      </c>
+      <c r="J29">
+        <v>0.4703164001761269</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1279,28 +1513,36 @@
         </is>
       </c>
       <c r="B30">
-        <v>0.1231424830617932</v>
+        <v>0.09932470154877088</v>
       </c>
       <c r="C30">
-        <v>0.1057617039478416</v>
+        <v>0.1648988055976923</v>
       </c>
       <c r="D30">
-        <v>0.3701484461121527</v>
+        <v>0.6120684661246356</v>
       </c>
       <c r="E30">
-        <v>0.7584405909654273</v>
+        <v>0.4609965909644891</v>
       </c>
       <c r="F30">
-        <v>0.7024405075804551</v>
+        <v>0.5764694574264668</v>
       </c>
       <c r="G30">
-        <v>1.109961385828214</v>
+        <v>0.2927841645363873</v>
       </c>
       <c r="H30">
-        <v>2.962192909170095</v>
+        <v>0.3150537121860421</v>
       </c>
       <c r="I30">
-        <v>4</v>
+        <v>1.0684105579979</v>
+      </c>
+      <c r="J30">
+        <v>1.090495924282298</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1310,28 +1552,36 @@
         </is>
       </c>
       <c r="B31">
-        <v>0.7075571816932016</v>
+        <v>0.6236975999832907</v>
       </c>
       <c r="C31">
-        <v>0.6035226596531975</v>
+        <v>0.6216705465803336</v>
       </c>
       <c r="D31">
-        <v>0.4946760023992498</v>
+        <v>0.5688493963950874</v>
       </c>
       <c r="E31">
-        <v>0.5902005758247939</v>
+        <v>0.5942489474564325</v>
       </c>
       <c r="F31">
-        <v>0.3537125468895475</v>
+        <v>0.315232804856797</v>
       </c>
       <c r="G31">
-        <v>1.258185359540162</v>
+        <v>0.6200357672849218</v>
       </c>
       <c r="H31">
-        <v>0.1673236168371306</v>
+        <v>0.7394758546210624</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>1.575701439226536</v>
+      </c>
+      <c r="J31">
+        <v>0.03864913669262049</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -1341,28 +1591,36 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.1057521479396167</v>
+        <v>0.0233008399365458</v>
       </c>
       <c r="C32">
-        <v>0.07797548950065247</v>
+        <v>0.1091206294878078</v>
       </c>
       <c r="D32">
-        <v>0.1503799197060093</v>
+        <v>0.7214397821161895</v>
       </c>
       <c r="E32">
-        <v>0.8343131984081218</v>
+        <v>0.1768740374266221</v>
       </c>
       <c r="F32">
-        <v>0.4793500051305901</v>
+        <v>0.5207012888977053</v>
       </c>
       <c r="G32">
-        <v>0.9827170266481504</v>
+        <v>0.1979918487758616</v>
       </c>
       <c r="H32">
-        <v>1.222860418629846</v>
+        <v>0.5188074069350315</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>1.069439925937441</v>
+      </c>
+      <c r="J32">
+        <v>1.089466556342757</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1372,28 +1630,36 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.1879086006493307</v>
+        <v>0.2608492539763008</v>
       </c>
       <c r="C33">
-        <v>0.3036341647311658</v>
+        <v>0.1557509510607723</v>
       </c>
       <c r="D33">
-        <v>0.4571751734861795</v>
+        <v>0.4299856081516526</v>
       </c>
       <c r="E33">
-        <v>0.4133574649520798</v>
+        <v>0.4890338886105928</v>
       </c>
       <c r="F33">
-        <v>0.2207514082056487</v>
+        <v>0.2066325108155346</v>
       </c>
       <c r="G33">
-        <v>0.7457265353321467</v>
+        <v>0.2240229135489698</v>
       </c>
       <c r="H33">
-        <v>0.6797824410451459</v>
+        <v>0.6786065684941789</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>1.034278779927258</v>
+      </c>
+      <c r="J33">
+        <v>1.12462770235294</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -1403,28 +1669,36 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.2167232123985194</v>
+        <v>0.2500339144193454</v>
       </c>
       <c r="C34">
-        <v>0.2346967824686141</v>
+        <v>0.2785091018318797</v>
       </c>
       <c r="D34">
-        <v>0.180761450625485</v>
+        <v>0.4060528162011625</v>
       </c>
       <c r="E34">
-        <v>0.5979393731024585</v>
+        <v>0.3078636088355367</v>
       </c>
       <c r="F34">
-        <v>0.6931487461821813</v>
+        <v>0.5850578262495393</v>
       </c>
       <c r="G34">
-        <v>0.9862620903014444</v>
+        <v>0.1697242431438572</v>
       </c>
       <c r="H34">
-        <v>3.085892204696864</v>
+        <v>0.369156712438243</v>
       </c>
       <c r="I34">
-        <v>4</v>
+        <v>0.9524278589258082</v>
+      </c>
+      <c r="J34">
+        <v>1.20647862335439</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -1434,28 +1708,36 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.03053246927454773</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.1052959967131368</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>0.7773477366301652</v>
       </c>
       <c r="E35">
-        <v>0.9133496754058943</v>
+        <v>0.07356523166023073</v>
       </c>
       <c r="F35">
-        <v>0.4546569519572882</v>
+        <v>0.4370785119013177</v>
       </c>
       <c r="G35">
-        <v>1.020711910975445</v>
+        <v>0.01318791659449812</v>
       </c>
       <c r="H35">
-        <v>1.184865534302551</v>
+        <v>0.5020062377462904</v>
       </c>
       <c r="I35">
-        <v>2</v>
+        <v>1.031499104858184</v>
+      </c>
+      <c r="J35">
+        <v>1.127407377422014</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1465,28 +1747,36 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.4338049198968876</v>
+        <v>0.3817154814733057</v>
       </c>
       <c r="C36">
-        <v>0.4373218364970234</v>
+        <v>0.3206560351384061</v>
       </c>
       <c r="D36">
-        <v>0.5437347406877751</v>
+        <v>0.5962494897157084</v>
       </c>
       <c r="E36">
-        <v>0.610709022408801</v>
+        <v>0.550370473495027</v>
       </c>
       <c r="F36">
-        <v>0.3385942414850379</v>
+        <v>0.3285819311290448</v>
       </c>
       <c r="G36">
-        <v>1.078283884630118</v>
+        <v>0.592694206779067</v>
       </c>
       <c r="H36">
-        <v>2.092524354306875</v>
+        <v>0.5234233108595495</v>
       </c>
       <c r="I36">
-        <v>3</v>
+        <v>1.280692228567659</v>
+      </c>
+      <c r="J36">
+        <v>0.2563600739662568</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -1496,28 +1786,36 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.2678292622464582</v>
+        <v>0.1834961714462366</v>
       </c>
       <c r="C37">
-        <v>0.2595149425888851</v>
+        <v>0.1699197824045043</v>
       </c>
       <c r="D37">
-        <v>0.6971563394202163</v>
+        <v>0.7944690507187741</v>
       </c>
       <c r="E37">
-        <v>0.7303325839378392</v>
+        <v>0.6351242659769474</v>
       </c>
       <c r="F37">
-        <v>0.1533816559037851</v>
+        <v>0.1891119950480841</v>
       </c>
       <c r="G37">
-        <v>1.087207016287744</v>
+        <v>0.4012577825926015</v>
       </c>
       <c r="H37">
-        <v>2.083601222649249</v>
+        <v>0.6180081217784049</v>
       </c>
       <c r="I37">
-        <v>3</v>
+        <v>1.294531836810836</v>
+      </c>
+      <c r="J37">
+        <v>1.863368589618293</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -1527,28 +1825,36 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.5374699926784561</v>
+        <v>0.5403975786781281</v>
       </c>
       <c r="C38">
-        <v>0.5724109765649704</v>
+        <v>0.4506192219849547</v>
       </c>
       <c r="D38">
-        <v>0.7793136478726639</v>
+        <v>0.6210948531928734</v>
       </c>
       <c r="E38">
-        <v>0.5694750332508369</v>
+        <v>0.8394827189929275</v>
       </c>
       <c r="F38">
-        <v>0.209711720122306</v>
+        <v>0.2159111485927669</v>
       </c>
       <c r="G38">
-        <v>1.261799865246125</v>
+        <v>0.262078538291417</v>
       </c>
       <c r="H38">
-        <v>0.1637091111311675</v>
+        <v>0.8537948520345212</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>1.558796238157575</v>
+      </c>
+      <c r="J38">
+        <v>0.02174393562365995</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -1558,28 +1864,36 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.3903587006423346</v>
+        <v>0.449344973037433</v>
       </c>
       <c r="C39">
-        <v>0.5158772635219858</v>
+        <v>0.2536458845402235</v>
       </c>
       <c r="D39">
-        <v>0.40584770554186</v>
+        <v>0.305420737225323</v>
       </c>
       <c r="E39">
-        <v>0.250039981392535</v>
+        <v>0.4064338111363375</v>
       </c>
       <c r="F39">
-        <v>0.2233709602612146</v>
+        <v>0.3019587601868651</v>
       </c>
       <c r="G39">
-        <v>0.8340480828240617</v>
+        <v>0.7699540444122277</v>
       </c>
       <c r="H39">
-        <v>0.5914608935532308</v>
+        <v>0.886970042024719</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>1.412601000958848</v>
+      </c>
+      <c r="J39">
+        <v>0.1244513015750675</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -1589,28 +1903,36 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.6304536524085928</v>
+        <v>0.6103263763221344</v>
       </c>
       <c r="C40">
-        <v>0.7022505929793724</v>
+        <v>0.4265671305772787</v>
       </c>
       <c r="D40">
-        <v>0.5155364227379119</v>
+        <v>0.5762385451143584</v>
       </c>
       <c r="E40">
-        <v>0.5846068903036332</v>
+        <v>0.4856868239771159</v>
       </c>
       <c r="F40">
-        <v>0.317957006286028</v>
+        <v>0.3796267374834196</v>
       </c>
       <c r="G40">
-        <v>1.264621437577853</v>
+        <v>0.9488348064471974</v>
       </c>
       <c r="H40">
-        <v>0.1608875387994395</v>
+        <v>0.5924508760493008</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>1.586758439288574</v>
+      </c>
+      <c r="J40">
+        <v>0.04970613675465851</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1620,28 +1942,36 @@
         </is>
       </c>
       <c r="B41">
-        <v>0.340385852010151</v>
+        <v>0.5089688175686381</v>
       </c>
       <c r="C41">
-        <v>0.5549919491277608</v>
+        <v>0.2564277641781311</v>
       </c>
       <c r="D41">
-        <v>0.495217641145805</v>
+        <v>0.2793339987304788</v>
       </c>
       <c r="E41">
-        <v>0.2128874400696618</v>
+        <v>0.446878236025805</v>
       </c>
       <c r="F41">
-        <v>0.09480932014783443</v>
+        <v>0.2177544391559399</v>
       </c>
       <c r="G41">
-        <v>0.8505462793250178</v>
+        <v>0.4430294794123464</v>
       </c>
       <c r="H41">
-        <v>0.5749626970522748</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>1.358758334502276</v>
+      </c>
+      <c r="J41">
+        <v>0.1782939680316391</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -1651,28 +1981,36 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.1126944077195089</v>
+        <v>0.1558941480709249</v>
       </c>
       <c r="C42">
-        <v>0.09788345592854511</v>
+        <v>0.2214290982170447</v>
       </c>
       <c r="D42">
-        <v>0.08654936204278145</v>
+        <v>0.559055597890242</v>
       </c>
       <c r="E42">
-        <v>0.7807038972705539</v>
+        <v>0.3541165273979129</v>
       </c>
       <c r="F42">
-        <v>0.8947622555126208</v>
+        <v>0.6227930976246179</v>
       </c>
       <c r="G42">
-        <v>1.19994585779911</v>
+        <v>0.2499148948348691</v>
       </c>
       <c r="H42">
-        <v>2.872208437199198</v>
+        <v>0.2507425875546221</v>
       </c>
       <c r="I42">
-        <v>4</v>
+        <v>1.012164042915734</v>
+      </c>
+      <c r="J42">
+        <v>1.146742439364464</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -1682,28 +2020,36 @@
         </is>
       </c>
       <c r="B43">
-        <v>0.287819128625246</v>
+        <v>0.7507477793827412</v>
       </c>
       <c r="C43">
-        <v>0.7935075731216946</v>
+        <v>0.1862550301752804</v>
       </c>
       <c r="D43">
-        <v>0.5105633163098777</v>
+        <v>0.5467364177378705</v>
       </c>
       <c r="E43">
-        <v>0.5387133090332767</v>
+        <v>0.5515204415729247</v>
       </c>
       <c r="F43">
-        <v>0.274804894324059</v>
+        <v>0.2796291761449021</v>
       </c>
       <c r="G43">
-        <v>1.157107937333185</v>
+        <v>0.4925229508587045</v>
       </c>
       <c r="H43">
-        <v>0.2684010390441076</v>
+        <v>0.828472192330807</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>1.486117821441759</v>
+      </c>
+      <c r="J43">
+        <v>0.05093448109215593</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -1713,28 +2059,36 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.3379922110463368</v>
+        <v>0.8601783694302829</v>
       </c>
       <c r="C44">
-        <v>0.8817607543554251</v>
+        <v>0.2557261268414058</v>
       </c>
       <c r="D44">
-        <v>0.3913375617878093</v>
+        <v>0.715354909943552</v>
       </c>
       <c r="E44">
-        <v>0.7701940493294157</v>
+        <v>0.5323002566525169</v>
       </c>
       <c r="F44">
-        <v>0.3397379611267418</v>
+        <v>0.2493326294303549</v>
       </c>
       <c r="G44">
-        <v>1.324200364661053</v>
+        <v>0.3430758299338398</v>
       </c>
       <c r="H44">
-        <v>0.1013086117162398</v>
+        <v>0.6632814465387015</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>1.490029849400222</v>
+      </c>
+      <c r="J44">
+        <v>0.04702245313369291</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -1744,28 +2098,36 @@
         </is>
       </c>
       <c r="B45">
-        <v>0.1302408605823024</v>
+        <v>0.6145144847130889</v>
       </c>
       <c r="C45">
-        <v>0.5414217555084808</v>
+        <v>0.1906520575410597</v>
       </c>
       <c r="D45">
-        <v>0.3073652346070889</v>
+        <v>0.6461602742541105</v>
       </c>
       <c r="E45">
-        <v>0.8264135118508165</v>
+        <v>0.2502502971852991</v>
       </c>
       <c r="F45">
-        <v>0.4250154133313393</v>
+        <v>0.2774259728663038</v>
       </c>
       <c r="G45">
-        <v>1.12613097847763</v>
+        <v>0.3114427313305368</v>
       </c>
       <c r="H45">
-        <v>1.079446466800367</v>
+        <v>0.1145281021971422</v>
       </c>
       <c r="I45">
-        <v>2</v>
+        <v>1.039809117936859</v>
+      </c>
+      <c r="J45">
+        <v>2.11809130849227</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1775,28 +2137,36 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.1198682035745439</v>
+        <v>0.4376704104626881</v>
       </c>
       <c r="C46">
-        <v>0.4164201406616568</v>
+        <v>0.1407938214517574</v>
       </c>
       <c r="D46">
-        <v>0.1928317845561923</v>
+        <v>0.814616667279416</v>
       </c>
       <c r="E46">
-        <v>0.9107150008645785</v>
+        <v>0.1637465001122176</v>
       </c>
       <c r="F46">
-        <v>0.1759571242661456</v>
+        <v>0.1125733506095943</v>
       </c>
       <c r="G46">
-        <v>1.041787377199287</v>
+        <v>0.130412623038166</v>
       </c>
       <c r="H46">
-        <v>1.16379006807871</v>
+        <v>0.3294760479343082</v>
       </c>
       <c r="I46">
-        <v>2</v>
+        <v>1.019816746744025</v>
+      </c>
+      <c r="J46">
+        <v>2.138083679685105</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1806,28 +2176,36 @@
         </is>
       </c>
       <c r="B47">
-        <v>0.3238590739894021</v>
+        <v>0.6978457440899401</v>
       </c>
       <c r="C47">
-        <v>0.7589642759235648</v>
+        <v>0.2058277402772046</v>
       </c>
       <c r="D47">
-        <v>0.6148553207368467</v>
+        <v>0.5678336597801</v>
       </c>
       <c r="E47">
-        <v>0.5982860487339937</v>
+        <v>0.6012243452982798</v>
       </c>
       <c r="F47">
-        <v>0.3404472815483584</v>
+        <v>0.3281439395694346</v>
       </c>
       <c r="G47">
-        <v>1.238066672273859</v>
+        <v>0.5337021887786528</v>
       </c>
       <c r="H47">
-        <v>0.1874423041034339</v>
+        <v>0.5625829860103244</v>
       </c>
       <c r="I47">
-        <v>1</v>
+        <v>1.386461541948509</v>
+      </c>
+      <c r="J47">
+        <v>0.1505907605854067</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -1837,28 +2215,36 @@
         </is>
       </c>
       <c r="B48">
-        <v>0.2625077706061623</v>
+        <v>0.4612567869644848</v>
       </c>
       <c r="C48">
-        <v>0.4931411824171468</v>
+        <v>0.2124773790026913</v>
       </c>
       <c r="D48">
-        <v>0.3598400883527819</v>
+        <v>0.4023549820246625</v>
       </c>
       <c r="E48">
-        <v>0.4756426966936041</v>
+        <v>0.3895274314147909</v>
       </c>
       <c r="F48">
-        <v>0.4707397454703294</v>
+        <v>0.4570952613069306</v>
       </c>
       <c r="G48">
-        <v>0.9430881864881838</v>
+        <v>0.5352310941898896</v>
       </c>
       <c r="H48">
-        <v>0.4824207898891088</v>
+        <v>0.5993189036326726</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>1.194201474560198</v>
+      </c>
+      <c r="J48">
+        <v>0.3428508279737175</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -1868,28 +2254,36 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.2730120295238055</v>
+        <v>0.3445233868168696</v>
       </c>
       <c r="C49">
-        <v>0.4041477675203857</v>
+        <v>0.1891648166787151</v>
       </c>
       <c r="D49">
-        <v>0.4761084537813239</v>
+        <v>0.7738123811422081</v>
       </c>
       <c r="E49">
-        <v>0.7242298944789988</v>
+        <v>0.5251024331048696</v>
       </c>
       <c r="F49">
-        <v>0.1339781504277696</v>
+        <v>0.1453308444442155</v>
       </c>
       <c r="G49">
-        <v>1.003498545523395</v>
+        <v>0.2719433385886524</v>
       </c>
       <c r="H49">
-        <v>2.167309693413597</v>
+        <v>0.7624493466513683</v>
       </c>
       <c r="I49">
-        <v>3</v>
+        <v>1.305910065185653</v>
+      </c>
+      <c r="J49">
+        <v>1.851990361243476</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1899,28 +2293,36 @@
         </is>
       </c>
       <c r="B50">
-        <v>0.2320624949043921</v>
+        <v>0.1926366977696411</v>
       </c>
       <c r="C50">
-        <v>0.2524913080024229</v>
+        <v>0.1870415856419982</v>
       </c>
       <c r="D50">
-        <v>0.6398893366428801</v>
+        <v>0.4191218178289837</v>
       </c>
       <c r="E50">
-        <v>0.387336429391719</v>
+        <v>0.6472835372693218</v>
       </c>
       <c r="F50">
-        <v>0.2427295276162471</v>
+        <v>0.2349721845081673</v>
       </c>
       <c r="G50">
-        <v>0.8579104606064802</v>
+        <v>0.2113921697269509</v>
       </c>
       <c r="H50">
-        <v>0.5675985157708123</v>
+        <v>0.642222727756559</v>
       </c>
       <c r="I50">
-        <v>1</v>
+        <v>1.085855025704954</v>
+      </c>
+      <c r="J50">
+        <v>1.073051456575244</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -1930,28 +2332,36 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.1863431917592368</v>
+        <v>0.144928280561572</v>
       </c>
       <c r="C51">
-        <v>0.1921485327891822</v>
+        <v>0.1163571725620709</v>
       </c>
       <c r="D51">
-        <v>0.6652668886681408</v>
+        <v>0.7983301059292705</v>
       </c>
       <c r="E51">
-        <v>0.7671103514926263</v>
+        <v>0.5929310379687344</v>
       </c>
       <c r="F51">
-        <v>0.2431336395509409</v>
+        <v>0.2222238170909572</v>
       </c>
       <c r="G51">
-        <v>1.077866937508833</v>
+        <v>0.4818053011315592</v>
       </c>
       <c r="H51">
-        <v>2.09294130142816</v>
+        <v>0.4693588881095576</v>
       </c>
       <c r="I51">
-        <v>3</v>
+        <v>1.235013729017326</v>
+      </c>
+      <c r="J51">
+        <v>1.922886697411803</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -1961,28 +2371,36 @@
         </is>
       </c>
       <c r="B52">
-        <v>0.3700990512264346</v>
+        <v>1</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0.3082599639222374</v>
       </c>
       <c r="D52">
-        <v>0.5467960768026011</v>
+        <v>0.5347149423526649</v>
       </c>
       <c r="E52">
-        <v>0.5909761633776248</v>
+        <v>0.5688496918179916</v>
       </c>
       <c r="F52">
-        <v>0.2774554322953927</v>
+        <v>0.2678712193038485</v>
       </c>
       <c r="G52">
-        <v>1.364622145473311</v>
+        <v>0.2764974073644421</v>
       </c>
       <c r="H52">
-        <v>0.06088683090398117</v>
+        <v>0.7428297803369266</v>
       </c>
       <c r="I52">
-        <v>1</v>
+        <v>1.550656678888003</v>
+      </c>
+      <c r="J52">
+        <v>0.01360437635408807</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -1992,28 +2410,36 @@
         </is>
       </c>
       <c r="B53">
-        <v>0.3183194858219158</v>
+        <v>0.580975135974304</v>
       </c>
       <c r="C53">
-        <v>0.6312491649169789</v>
+        <v>0.2034840982701519</v>
       </c>
       <c r="D53">
-        <v>0.3976881672030233</v>
+        <v>0.3840006938727135</v>
       </c>
       <c r="E53">
-        <v>0.3872373925475159</v>
+        <v>0.4213898932594803</v>
       </c>
       <c r="F53">
-        <v>0.318036754257141</v>
+        <v>0.3255256395618579</v>
       </c>
       <c r="G53">
-        <v>0.9534457807557952</v>
+        <v>0.6841928447670084</v>
       </c>
       <c r="H53">
-        <v>0.4720631956214973</v>
+        <v>0.7151651753418555</v>
       </c>
       <c r="I53">
-        <v>1</v>
+        <v>1.33772638486703</v>
+      </c>
+      <c r="J53">
+        <v>0.1993259176668849</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -2023,28 +2449,36 @@
         </is>
       </c>
       <c r="B54">
-        <v>0.150112643480478</v>
+        <v>0.185138468115493</v>
       </c>
       <c r="C54">
-        <v>0.2093821482464568</v>
+        <v>0.148008737118851</v>
       </c>
       <c r="D54">
-        <v>0.225770471687149</v>
+        <v>0.2849457943244343</v>
       </c>
       <c r="E54">
-        <v>0.3101053765036838</v>
+        <v>0.2782424232570102</v>
       </c>
       <c r="F54">
-        <v>0.2359801604177216</v>
+        <v>0.1896813048463396</v>
       </c>
       <c r="G54">
-        <v>0.5188438842947859</v>
+        <v>0.2068337252630412</v>
       </c>
       <c r="H54">
-        <v>0.9066650920825067</v>
+        <v>0.5542488256395411</v>
       </c>
       <c r="I54">
-        <v>1</v>
+        <v>0.7750785369754424</v>
+      </c>
+      <c r="J54">
+        <v>1.383827945304756</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -2054,28 +2488,36 @@
         </is>
       </c>
       <c r="B55">
-        <v>0.6227540638156141</v>
+        <v>0.4761514378208396</v>
       </c>
       <c r="C55">
-        <v>0.5099967048769454</v>
+        <v>0.482095838500992</v>
       </c>
       <c r="D55">
-        <v>0.4594574195369656</v>
+        <v>0.5571380318367922</v>
       </c>
       <c r="E55">
-        <v>0.6119710371068492</v>
+        <v>0.3753648312556153</v>
       </c>
       <c r="F55">
-        <v>0.3670074785220746</v>
+        <v>0.3848195573197211</v>
       </c>
       <c r="G55">
-        <v>1.169710828752361</v>
+        <v>1</v>
       </c>
       <c r="H55">
-        <v>0.2557981476249316</v>
+        <v>0.3827712780739148</v>
       </c>
       <c r="I55">
-        <v>1</v>
+        <v>1.484937061061998</v>
+      </c>
+      <c r="J55">
+        <v>0.05211524147191771</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -2085,28 +2527,36 @@
         </is>
       </c>
       <c r="B56">
-        <v>0.09967866617435159</v>
+        <v>0.1019793861375826</v>
       </c>
       <c r="C56">
-        <v>0.1459494737541952</v>
+        <v>0.05514970382902217</v>
       </c>
       <c r="D56">
-        <v>0.1455643155131141</v>
+        <v>0.9473200069135406</v>
       </c>
       <c r="E56">
-        <v>0.9314630996666015</v>
+        <v>0.1535280076616485</v>
       </c>
       <c r="F56">
-        <v>0.1061489979652205</v>
+        <v>0.1227727244764361</v>
       </c>
       <c r="G56">
-        <v>0.965047755885562</v>
+        <v>0.3472489092140805</v>
       </c>
       <c r="H56">
-        <v>1.240529689392435</v>
+        <v>0.6223191540767408</v>
       </c>
       <c r="I56">
-        <v>2</v>
+        <v>1.207213073993642</v>
+      </c>
+      <c r="J56">
+        <v>1.950687352435487</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -2116,28 +2566,36 @@
         </is>
       </c>
       <c r="B57">
-        <v>0.1893241263354704</v>
+        <v>0.1228061399094799</v>
       </c>
       <c r="C57">
-        <v>0.128207774228103</v>
+        <v>0.252710861668575</v>
       </c>
       <c r="D57">
-        <v>0.167379877901918</v>
+        <v>0.5076924117869736</v>
       </c>
       <c r="E57">
-        <v>0.663802681096796</v>
+        <v>0.2699633811148243</v>
       </c>
       <c r="F57">
-        <v>0.6099584859791144</v>
+        <v>0.5998010205970541</v>
       </c>
       <c r="G57">
-        <v>0.9449763149205923</v>
+        <v>0.04621669690621268</v>
       </c>
       <c r="H57">
-        <v>3.127177980077716</v>
+        <v>0.5758814514244628</v>
       </c>
       <c r="I57">
-        <v>4</v>
+        <v>1.050291689584706</v>
+      </c>
+      <c r="J57">
+        <v>1.108614792695492</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -2147,28 +2605,36 @@
         </is>
       </c>
       <c r="B58">
-        <v>0.8882750395112022</v>
+        <v>0.5045440332448137</v>
       </c>
       <c r="C58">
-        <v>0.4477779176289458</v>
+        <v>0.8537645634009498</v>
       </c>
       <c r="D58">
-        <v>0.6384372929759447</v>
+        <v>0.4930665392004509</v>
       </c>
       <c r="E58">
-        <v>0.5029392371926392</v>
+        <v>0.6675131780084531</v>
       </c>
       <c r="F58">
-        <v>0.2082897462758141</v>
+        <v>0.2213973813099903</v>
       </c>
       <c r="G58">
-        <v>1.30133480746069</v>
+        <v>0.3319537720720917</v>
       </c>
       <c r="H58">
-        <v>0.1241741689166023</v>
+        <v>0.7485820817583977</v>
       </c>
       <c r="I58">
-        <v>1</v>
+        <v>1.546529115946338</v>
+      </c>
+      <c r="J58">
+        <v>0.009476813412422347</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -2178,28 +2644,36 @@
         </is>
       </c>
       <c r="B59">
-        <v>0.5684225895050638</v>
+        <v>0.489282344218021</v>
       </c>
       <c r="C59">
-        <v>0.5486635544640451</v>
+        <v>0.4571200502910165</v>
       </c>
       <c r="D59">
-        <v>0.8474970446694069</v>
+        <v>0.698634409573226</v>
       </c>
       <c r="E59">
-        <v>0.6026942438035161</v>
+        <v>1</v>
       </c>
       <c r="F59">
-        <v>0.1870990799881795</v>
+        <v>0.1767145823462854</v>
       </c>
       <c r="G59">
-        <v>1.319330737240081</v>
+        <v>0.1253376029544824</v>
       </c>
       <c r="H59">
-        <v>0.1061782391372113</v>
+        <v>0.9708211824378412</v>
       </c>
       <c r="I59">
-        <v>1</v>
+        <v>1.71051960455865</v>
+      </c>
+      <c r="J59">
+        <v>0.1734673020247344</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -2209,28 +2683,36 @@
         </is>
       </c>
       <c r="B60">
-        <v>0.09706043702595729</v>
+        <v>0.3108046243843088</v>
       </c>
       <c r="C60">
-        <v>0.35146101151432</v>
+        <v>0.04383690129334691</v>
       </c>
       <c r="D60">
-        <v>0.7355076168920529</v>
+        <v>0.7463237747024459</v>
       </c>
       <c r="E60">
-        <v>0.7534262397176739</v>
+        <v>0.6222352549787773</v>
       </c>
       <c r="F60">
-        <v>0.3076642662344015</v>
+        <v>0.293225052457977</v>
       </c>
       <c r="G60">
-        <v>1.155952172440206</v>
+        <v>0.4048025451475676</v>
       </c>
       <c r="H60">
-        <v>2.014856066496786</v>
+        <v>0.4366300137383708</v>
       </c>
       <c r="I60">
-        <v>3</v>
+        <v>1.217862421836879</v>
+      </c>
+      <c r="J60">
+        <v>1.940038004592251</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -2240,28 +2722,36 @@
         </is>
       </c>
       <c r="B61">
-        <v>0.5096463975090511</v>
+        <v>0.625456547522516</v>
       </c>
       <c r="C61">
-        <v>0.6850904522550292</v>
+        <v>0.3565921376153795</v>
       </c>
       <c r="D61">
-        <v>0.4929723360336532</v>
+        <v>0.5226486429044899</v>
       </c>
       <c r="E61">
-        <v>0.5253680844751781</v>
+        <v>0.506021757219201</v>
       </c>
       <c r="F61">
-        <v>0.3211900574852541</v>
+        <v>0.3456194677104331</v>
       </c>
       <c r="G61">
-        <v>1.16244775348053</v>
+        <v>0.7920334905855517</v>
       </c>
       <c r="H61">
-        <v>0.263061222896763</v>
+        <v>0.6835612706661469</v>
       </c>
       <c r="I61">
-        <v>1</v>
+        <v>1.503861478189164</v>
+      </c>
+      <c r="J61">
+        <v>0.03319082434475118</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -2271,28 +2761,36 @@
         </is>
       </c>
       <c r="B62">
-        <v>0.1503741314603009</v>
+        <v>0.1419126372858185</v>
       </c>
       <c r="C62">
-        <v>0.181300446088326</v>
+        <v>0.1103999128125059</v>
       </c>
       <c r="D62">
-        <v>0.5439766258941465</v>
+        <v>0.8285313336589671</v>
       </c>
       <c r="E62">
-        <v>0.79743832628943</v>
+        <v>0.4875333007979525</v>
       </c>
       <c r="F62">
-        <v>0.1420598781496164</v>
+        <v>0.1425315552457795</v>
       </c>
       <c r="G62">
-        <v>1.003733876034189</v>
+        <v>0.2695080143959858</v>
       </c>
       <c r="H62">
-        <v>2.167074362902803</v>
+        <v>0.5450575613307365</v>
       </c>
       <c r="I62">
-        <v>3</v>
+        <v>1.16039553034314</v>
+      </c>
+      <c r="J62">
+        <v>1.99750489608599</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -2302,28 +2800,36 @@
         </is>
       </c>
       <c r="B63">
-        <v>0.2354626739934722</v>
+        <v>0.1683276967618195</v>
       </c>
       <c r="C63">
-        <v>0.2505109069448988</v>
+        <v>0.136852576584014</v>
       </c>
       <c r="D63">
-        <v>0.6003432772618731</v>
+        <v>0.6913087782760082</v>
       </c>
       <c r="E63">
-        <v>0.6691679981443229</v>
+        <v>0.547869013829473</v>
       </c>
       <c r="F63">
-        <v>0.2386360545424719</v>
+        <v>0.2346511550058448</v>
       </c>
       <c r="G63">
-        <v>0.9916367339727368</v>
+        <v>0.4890316787269002</v>
       </c>
       <c r="H63">
-        <v>2.179171504964256</v>
+        <v>0.4516822718312574</v>
       </c>
       <c r="I63">
-        <v>3</v>
+        <v>1.150374350583949</v>
+      </c>
+      <c r="J63">
+        <v>2.00752607584518</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -2333,28 +2839,36 @@
         </is>
       </c>
       <c r="B64">
-        <v>0.4212834121838566</v>
+        <v>0.6602289176487198</v>
       </c>
       <c r="C64">
-        <v>0.6937824745143233</v>
+        <v>0.3195860898786126</v>
       </c>
       <c r="D64">
-        <v>0.5138067738594548</v>
+        <v>0.6097119631419834</v>
       </c>
       <c r="E64">
-        <v>0.676172317885387</v>
+        <v>0.5517112353992263</v>
       </c>
       <c r="F64">
-        <v>0.3910655783632627</v>
+        <v>0.32731079829958</v>
       </c>
       <c r="G64">
-        <v>1.238124600451603</v>
+        <v>0.5240782383405759</v>
       </c>
       <c r="H64">
-        <v>0.1873843759256895</v>
+        <v>0.4499765969797459</v>
       </c>
       <c r="I64">
-        <v>1</v>
+        <v>1.341059564010054</v>
+      </c>
+      <c r="J64">
+        <v>0.1959927385238618</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -2364,28 +2878,36 @@
         </is>
       </c>
       <c r="B65">
-        <v>0.4061676762177369</v>
+        <v>0.3264953227065793</v>
       </c>
       <c r="C65">
-        <v>0.3454110091824543</v>
+        <v>0.3645377657184441</v>
       </c>
       <c r="D65">
-        <v>0.4249709575346669</v>
+        <v>0.640293709794982</v>
       </c>
       <c r="E65">
-        <v>0.6825303026795034</v>
+        <v>0.5050344102852989</v>
       </c>
       <c r="F65">
-        <v>0.3144486520249263</v>
+        <v>0.2459034875262259</v>
       </c>
       <c r="G65">
-        <v>1.014695437090636</v>
+        <v>0.2762514863415604</v>
       </c>
       <c r="H65">
-        <v>2.156112801846356</v>
+        <v>0.497582192457303</v>
       </c>
       <c r="I65">
-        <v>3</v>
+        <v>1.135294770486329</v>
+      </c>
+      <c r="J65">
+        <v>2.0226056559428</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -2395,28 +2917,36 @@
         </is>
       </c>
       <c r="B66">
-        <v>0.3884966918231512</v>
+        <v>0.5905917418243416</v>
       </c>
       <c r="C66">
-        <v>0.67039253953159</v>
+        <v>0.2375950183783203</v>
       </c>
       <c r="D66">
-        <v>0.4725262246732364</v>
+        <v>0.4533952361855207</v>
       </c>
       <c r="E66">
-        <v>0.4322721652501644</v>
+        <v>0.5107851828093548</v>
       </c>
       <c r="F66">
-        <v>0.2820519891192763</v>
+        <v>0.3138221351080539</v>
       </c>
       <c r="G66">
-        <v>1.044054318049255</v>
+        <v>0.6550570906725204</v>
       </c>
       <c r="H66">
-        <v>0.3814546583280376</v>
+        <v>0.7685227682029312</v>
       </c>
       <c r="I66">
-        <v>1</v>
+        <v>1.410648826325331</v>
+      </c>
+      <c r="J66">
+        <v>0.1264034762085839</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -2426,28 +2956,36 @@
         </is>
       </c>
       <c r="B67">
-        <v>0.1345409143808791</v>
+        <v>0.03663850106851675</v>
       </c>
       <c r="C67">
-        <v>0.02200615646268134</v>
+        <v>0.2118623514725264</v>
       </c>
       <c r="D67">
-        <v>0.04370690528901593</v>
+        <v>0.7117787682020734</v>
       </c>
       <c r="E67">
-        <v>0.8445558376414979</v>
+        <v>0.1227136979294389</v>
       </c>
       <c r="F67">
-        <v>0.441536857056563</v>
+        <v>0.4237107020425084</v>
       </c>
       <c r="G67">
-        <v>0.9637038866624779</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>1.241873558615519</v>
+        <v>0.5278032356404918</v>
       </c>
       <c r="I67">
-        <v>2</v>
+        <v>1.012927794481286</v>
+      </c>
+      <c r="J67">
+        <v>1.145978687798912</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -2457,28 +2995,36 @@
         </is>
       </c>
       <c r="B68">
-        <v>0.1849786713066997</v>
+        <v>0.1778377422639517</v>
       </c>
       <c r="C68">
-        <v>0.2077735030918338</v>
+        <v>0.1421613604954913</v>
       </c>
       <c r="D68">
-        <v>0.6261743685293989</v>
+        <v>0.76018410440178</v>
       </c>
       <c r="E68">
-        <v>0.7586386562948208</v>
+        <v>0.6446470741683262</v>
       </c>
       <c r="F68">
-        <v>0.3316680160820311</v>
+        <v>0.2257955006594133</v>
       </c>
       <c r="G68">
-        <v>1.074717433070311</v>
+        <v>0.3846615032109729</v>
       </c>
       <c r="H68">
-        <v>2.096090805866682</v>
+        <v>0.4057550113869175</v>
       </c>
       <c r="I68">
-        <v>3</v>
+        <v>1.186958738645344</v>
+      </c>
+      <c r="J68">
+        <v>1.970941687783785</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -2488,28 +3034,36 @@
         </is>
       </c>
       <c r="B69">
-        <v>0.4060376717574559</v>
+        <v>0.5602474741921381</v>
       </c>
       <c r="C69">
-        <v>0.5745794926220353</v>
+        <v>0.3512511330403388</v>
       </c>
       <c r="D69">
-        <v>0.4877154742285955</v>
+        <v>0.2883863718360964</v>
       </c>
       <c r="E69">
-        <v>0.3088705813145832</v>
+        <v>0.3971871642092361</v>
       </c>
       <c r="F69">
-        <v>0.1793232598620332</v>
+        <v>0.2546977040223207</v>
       </c>
       <c r="G69">
-        <v>0.927594973875554</v>
+        <v>0.4054520051770287</v>
       </c>
       <c r="H69">
-        <v>0.4979140025017386</v>
+        <v>0.6860546949617629</v>
       </c>
       <c r="I69">
-        <v>1</v>
+        <v>1.173930247966014</v>
+      </c>
+      <c r="J69">
+        <v>0.3631220545679017</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -2519,28 +3073,36 @@
         </is>
       </c>
       <c r="B70">
-        <v>0.08497333083415525</v>
+        <v>0.3513177607091415</v>
       </c>
       <c r="C70">
-        <v>0.312896151083146</v>
+        <v>0.1396226349958548</v>
       </c>
       <c r="D70">
-        <v>0.2799520096964024</v>
+        <v>0.7667488597209243</v>
       </c>
       <c r="E70">
-        <v>0.8639302350655507</v>
+        <v>0.1494799371354843</v>
       </c>
       <c r="F70">
-        <v>0.1674794941168471</v>
+        <v>0.1530721713710249</v>
       </c>
       <c r="G70">
-        <v>0.978735116391971</v>
+        <v>0.1522958032126125</v>
       </c>
       <c r="H70">
-        <v>1.226842328886026</v>
+        <v>0.3276354035555776</v>
       </c>
       <c r="I70">
-        <v>2</v>
+        <v>0.9524372807012956</v>
+      </c>
+      <c r="J70">
+        <v>2.205463145727833</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="71">
@@ -2550,28 +3112,36 @@
         </is>
       </c>
       <c r="B71">
-        <v>0.2857915354196733</v>
+        <v>0.4025332097662377</v>
       </c>
       <c r="C71">
-        <v>0.3924377365976181</v>
+        <v>0.2630789570899246</v>
       </c>
       <c r="D71">
-        <v>0.565761709887228</v>
+        <v>0.5490958325040828</v>
       </c>
       <c r="E71">
-        <v>0.6851590727509931</v>
+        <v>0.6243443230287051</v>
       </c>
       <c r="F71">
-        <v>0.5981917852928398</v>
+        <v>0.3622761054379839</v>
       </c>
       <c r="G71">
-        <v>1.176030126383993</v>
+        <v>0.4865905379355301</v>
       </c>
       <c r="H71">
-        <v>1.994778112552999</v>
+        <v>0</v>
       </c>
       <c r="I71">
-        <v>3</v>
+        <v>1.136032533768051</v>
+      </c>
+      <c r="J71">
+        <v>2.021867892661078</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="72">
@@ -2581,28 +3151,36 @@
         </is>
       </c>
       <c r="B72">
-        <v>0.2523522082434229</v>
+        <v>0.3145048262822661</v>
       </c>
       <c r="C72">
-        <v>0.2982500285848334</v>
+        <v>0.2653256198620546</v>
       </c>
       <c r="D72">
-        <v>0.194631056567987</v>
+        <v>0.4228588507749025</v>
       </c>
       <c r="E72">
-        <v>0.5945983133642823</v>
+        <v>0.4815965932063323</v>
       </c>
       <c r="F72">
-        <v>0.7555544794136481</v>
+        <v>0.4335625279258913</v>
       </c>
       <c r="G72">
-        <v>1.055900416873975</v>
+        <v>0.3747009206367044</v>
       </c>
       <c r="H72">
-        <v>3.016253878124334</v>
+        <v>0.1204531554152263</v>
       </c>
       <c r="I72">
-        <v>4</v>
+        <v>0.9606987377807917</v>
+      </c>
+      <c r="J72">
+        <v>2.197201688648337</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="73">
@@ -2612,28 +3190,36 @@
         </is>
       </c>
       <c r="B73">
-        <v>0.3070683902740563</v>
+        <v>0.5892481163290954</v>
       </c>
       <c r="C73">
-        <v>0.6430467353151093</v>
+        <v>0.1989776049323213</v>
       </c>
       <c r="D73">
-        <v>0.5518087855954398</v>
+        <v>0.5118882565511091</v>
       </c>
       <c r="E73">
-        <v>0.5101837753267817</v>
+        <v>0.496506393814708</v>
       </c>
       <c r="F73">
-        <v>0.259665039330444</v>
+        <v>0.3010832398932561</v>
       </c>
       <c r="G73">
-        <v>1.067710847197126</v>
+        <v>0.5960862571936548</v>
       </c>
       <c r="H73">
-        <v>0.3577981291801671</v>
+        <v>0.6780706111259097</v>
       </c>
       <c r="I73">
-        <v>1</v>
+        <v>1.342051904058943</v>
+      </c>
+      <c r="J73">
+        <v>0.1950003984749722</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -2643,28 +3229,36 @@
         </is>
       </c>
       <c r="B74">
-        <v>0.290336235004472</v>
+        <v>0.5149626095925405</v>
       </c>
       <c r="C74">
-        <v>0.5499790669724742</v>
+        <v>0.2155666038666756</v>
       </c>
       <c r="D74">
-        <v>0.4828774060466415</v>
+        <v>0.4705903472177256</v>
       </c>
       <c r="E74">
-        <v>0.4802102259937983</v>
+        <v>0.3883914998517252</v>
       </c>
       <c r="F74">
-        <v>0.2020751201876781</v>
+        <v>0.2617511991400962</v>
       </c>
       <c r="G74">
-        <v>0.9441286501757574</v>
+        <v>0.515937529939953</v>
       </c>
       <c r="H74">
-        <v>0.4813803262015352</v>
+        <v>0.6418856099531477</v>
       </c>
       <c r="I74">
-        <v>1</v>
+        <v>1.196110798943512</v>
+      </c>
+      <c r="J74">
+        <v>0.3409415035904035</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>